<commit_message>
updated with new temp sensor
</commit_message>
<xml_diff>
--- a/MAIN/Prototype_001_Schematic/PrototypePinout.xlsx
+++ b/MAIN/Prototype_001_Schematic/PrototypePinout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mason\Documents\Arduino\HeatShield-Biometrics-Prototype\MAIN\Prototype_001_Schematic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B72A16ED-7666-44F0-9B99-98FADE962191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCDEE64-2960-4A2D-8A8E-4DD84E1A8D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FB7C1E7B-28C9-4D8E-A399-8BEE433A4DC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="61">
   <si>
     <t>Peripheral</t>
   </si>
@@ -192,6 +192,33 @@
   </si>
   <si>
     <t>D9</t>
+  </si>
+  <si>
+    <t>Vdd</t>
+  </si>
+  <si>
+    <t>Gnd</t>
+  </si>
+  <si>
+    <t>Alert</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>2.7-5.5V</t>
+  </si>
+  <si>
+    <t>already pull-up resistor on board</t>
+  </si>
+  <si>
+    <t>lower 3 bits of I2C address</t>
   </si>
 </sst>
 </file>
@@ -221,7 +248,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,6 +258,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -247,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -265,10 +298,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -279,6 +312,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -614,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{776CDE91-EEF9-4DE3-B987-D33A9D6BE5CD}">
-  <dimension ref="A1:O41"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1290,13 +1329,13 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1313,7 +1352,7 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>3</v>
@@ -1340,7 +1379,7 @@
         <v>36</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -1363,7 +1402,7 @@
         <v>9</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -1380,7 +1419,7 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="4" t="s">
@@ -1401,11 +1440,13 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B37" s="5"/>
+        <v>55</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="C37" s="4" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -1421,9 +1462,15 @@
       <c r="O37" s="1"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
+      <c r="A38" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -1438,14 +1485,14 @@
       <c r="O38" s="1"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>12</v>
+      <c r="A39" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -1461,15 +1508,6 @@
       <c r="O39" s="1"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -1484,13 +1522,106 @@
       <c r="O40" s="1"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B43" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C41" s="8"/>
+      <c r="C43" s="8"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" s="4"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B50" s="5"/>
+      <c r="C50" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B51" s="5"/>
+      <c r="C51" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added haptic feedback vibration motor
</commit_message>
<xml_diff>
--- a/MAIN/Prototype_001_Schematic/PrototypePinout.xlsx
+++ b/MAIN/Prototype_001_Schematic/PrototypePinout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mason\Documents\Arduino\HeatShield-Biometrics-Prototype\MAIN\Prototype_001_Schematic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AD203D-7694-4F29-9587-E4B783AE23E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F4CBD7-4534-47F3-9D09-4C06BAA486B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FB7C1E7B-28C9-4D8E-A399-8BEE433A4DC3}"/>
+    <workbookView xWindow="3690" yWindow="1755" windowWidth="21600" windowHeight="11295" xr2:uid="{FB7C1E7B-28C9-4D8E-A399-8BEE433A4DC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="65">
   <si>
     <t>Peripheral</t>
   </si>
@@ -219,6 +219,18 @@
   </si>
   <si>
     <t>lower 3 bits of I2C address</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>Control (NPN)</t>
+  </si>
+  <si>
+    <t>VBAT</t>
+  </si>
+  <si>
+    <t>connect to npn transistor</t>
   </si>
 </sst>
 </file>
@@ -280,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -297,12 +309,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -653,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{776CDE91-EEF9-4DE3-B987-D33A9D6BE5CD}">
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,13 +673,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D1" s="1"/>
@@ -707,13 +713,13 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="1"/>
@@ -921,13 +927,13 @@
       <c r="O12" s="1"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="1"/>
@@ -1137,13 +1143,13 @@
       <c r="O22" s="1"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D23" s="1"/>
@@ -1305,13 +1311,13 @@
       <c r="O30" s="1"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D31" s="1"/>
@@ -1508,6 +1514,9 @@
       <c r="O39" s="1"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -1522,13 +1531,13 @@
       <c r="O40" s="1"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C41" s="9" t="s">
+      <c r="C41" s="7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1537,69 +1546,74 @@
         <v>26</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C43" s="8"/>
+      <c r="C43" s="3"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" s="12" t="s">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B45" s="13" t="s">
+      <c r="B46" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="13" t="s">
+      <c r="C46" s="11" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C47" s="4"/>
+        <v>48</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>37</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="4"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>37</v>
@@ -1607,19 +1621,30 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B50" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="C50" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B52" s="5"/>
+      <c r="C52" s="4" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added hella code shit and im fuckin tired
</commit_message>
<xml_diff>
--- a/MAIN/Prototype_001_Schematic/PrototypePinout.xlsx
+++ b/MAIN/Prototype_001_Schematic/PrototypePinout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mason\Documents\Arduino\HeatShield-Biometrics-Prototype\MAIN\Prototype_001_Schematic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F4CBD7-4534-47F3-9D09-4C06BAA486B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC3433A-9518-4E6D-8E74-BA273BDC72DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3690" yWindow="1755" windowWidth="21600" windowHeight="11295" xr2:uid="{FB7C1E7B-28C9-4D8E-A399-8BEE433A4DC3}"/>
+    <workbookView xWindow="-28920" yWindow="-5850" windowWidth="29040" windowHeight="15720" xr2:uid="{FB7C1E7B-28C9-4D8E-A399-8BEE433A4DC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="65">
   <si>
     <t>Peripheral</t>
   </si>
@@ -95,9 +95,6 @@
     <t>NSS</t>
   </si>
   <si>
-    <t>DIO 0-4</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 5 digital I/O pins, software configured</t>
   </si>
   <si>
@@ -231,6 +228,9 @@
   </si>
   <si>
     <t>connect to npn transistor</t>
+  </si>
+  <si>
+    <t>G0</t>
   </si>
 </sst>
 </file>
@@ -260,7 +260,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -279,6 +279,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -292,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -324,6 +330,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -661,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{776CDE91-EEF9-4DE3-B987-D33A9D6BE5CD}">
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,7 +749,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>14</v>
@@ -847,7 +856,7 @@
         <v>18</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>15</v>
@@ -870,7 +879,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>16</v>
@@ -890,11 +899,13 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -951,13 +962,13 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1037,13 +1048,13 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>51</v>
+        <v>21</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>50</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1060,13 +1071,13 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1083,13 +1094,13 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1106,11 +1117,11 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1170,7 +1181,7 @@
         <v>13</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>14</v>
@@ -1211,11 +1222,11 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1232,11 +1243,11 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1253,11 +1264,11 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -1274,11 +1285,11 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1335,13 +1346,13 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1358,7 +1369,7 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>3</v>
@@ -1379,13 +1390,13 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -1408,7 +1419,7 @@
         <v>9</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -1425,11 +1436,11 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -1446,13 +1457,13 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -1469,13 +1480,13 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -1492,13 +1503,13 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -1532,7 +1543,7 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>1</v>
@@ -1543,13 +1554,13 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
@@ -1563,13 +1574,13 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
@@ -1590,13 +1601,13 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C47" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
@@ -1610,13 +1621,13 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C49" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1627,25 +1638,25 @@
         <v>9</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>